<commit_message>
update loyn data file
</commit_message>
<xml_diff>
--- a/data/loyn.xlsx
+++ b/data/loyn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhy163/Documents/Alex/Teaching/BI5009_repo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhy163/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A793630-7FBC-A04B-95E7-AA13553E53FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{548DCE99-0754-B04D-B3EC-B501BE210D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,12 +71,14 @@
       <sz val="9"/>
       <color indexed="10"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="48"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -527,7 +529,7 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD726"/>
+      <selection activeCell="I1" sqref="I1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.19921875" defaultRowHeight="12" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
update GDE and LM1 exercises
</commit_message>
<xml_diff>
--- a/data/loyn.xlsx
+++ b/data/loyn.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhy163/Documents/Alex/Teaching/PGR-LM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E204EE04-1909-C34B-ADF9-31E51CBF0C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608E7413-42C2-1342-ADE1-8707AF2FB2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loyn_up" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -883,11 +883,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:XFD184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>